<commit_message>
added priority and packages to test json file
</commit_message>
<xml_diff>
--- a/app/data/Reference Data for CS Mid Tier and Higher Tier Options and Capital Items.xlsx
+++ b/app/data/Reference Data for CS Mid Tier and Higher Tier Options and Capital Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattfielding/projects/defra/local-nature-recovery-prototype/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF8EF25-3D3D-B44E-A46D-AD8A26A2B032}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46D25AC-1AD7-CA4B-A383-652858381792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="1020" windowWidth="50820" windowHeight="26200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54840" yWindow="8100" windowWidth="24460" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="1047">
   <si>
     <t>Option</t>
   </si>
@@ -2810,9 +2810,6 @@
 trees forming distinctive features in the landscape
 trees providing valuable habitat
 areas under tree canopies free from scrub, soil compaction, or anything which threatens the tree’s longevity</t>
-  </si>
-  <si>
-    <t>priorty</t>
   </si>
   <si>
     <t>https://www.gov.uk/countryside-stewardship-grants/hedgerow-supplement-substantial-pre-work-bn9</t>
@@ -3150,9 +3147,6 @@
   </si>
   <si>
     <t>package</t>
-  </si>
-  <si>
-    <t>polinators, water</t>
   </si>
   <si>
     <r>
@@ -3593,6 +3587,18 @@
   </si>
   <si>
     <t xml:space="preserve">AB1 Nectar flower mix </t>
+  </si>
+  <si>
+    <t>Pollinators and Wildlife,Improving Water Quality</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Pollinators and Wildlife</t>
+  </si>
+  <si>
+    <t>priority</t>
   </si>
 </sst>
 </file>
@@ -4453,8 +4459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4502,13 +4508,13 @@
         <v>867</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>924</v>
+        <v>1046</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>851</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>849</v>
@@ -4551,8 +4557,8 @@
       <c r="K2" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>1024</v>
+      <c r="L2" t="s">
+        <v>1043</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>0</v>
@@ -4592,8 +4598,8 @@
       <c r="K3" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>1024</v>
+      <c r="L3" t="s">
+        <v>1044</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>0</v>
@@ -4633,8 +4639,8 @@
       <c r="K4" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>1024</v>
+      <c r="L4" t="s">
+        <v>1045</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>0</v>
@@ -4670,6 +4676,9 @@
       </c>
       <c r="H5" s="3" t="s">
         <v>920</v>
+      </c>
+      <c r="J5" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>568</v>
@@ -5458,7 +5467,7 @@
         <v>923</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5517,7 +5526,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>578</v>
@@ -5555,7 +5564,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>579</v>
@@ -5593,7 +5602,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>579</v>
@@ -5631,7 +5640,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>580</v>
@@ -5669,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>581</v>
@@ -5707,7 +5716,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>580</v>
@@ -5745,7 +5754,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>578</v>
@@ -5783,7 +5792,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>578</v>
@@ -5821,7 +5830,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>578</v>
@@ -5859,7 +5868,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>579</v>
@@ -5897,7 +5906,7 @@
         <v>1</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>579</v>
@@ -5935,7 +5944,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>582</v>
@@ -5973,7 +5982,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>579</v>
@@ -6011,7 +6020,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>579</v>
@@ -6020,10 +6029,10 @@
         <v>605</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -6061,10 +6070,10 @@
         <v>0</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O41" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="1" customFormat="1" ht="204" x14ac:dyDescent="0.2">
@@ -6102,10 +6111,10 @@
         <v>0</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="O42" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="1" customFormat="1" ht="340" x14ac:dyDescent="0.2">
@@ -6143,10 +6152,10 @@
         <v>0</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="O43" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -6184,10 +6193,10 @@
         <v>0</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="O44" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -6222,10 +6231,10 @@
         <v>0</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="O45" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -6260,10 +6269,10 @@
         <v>604</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="O46" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -6298,10 +6307,10 @@
         <v>0</v>
       </c>
       <c r="N47" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="O47" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -6359,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>583</v>
@@ -6397,7 +6406,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>629</v>
@@ -6406,10 +6415,10 @@
         <v>605</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="O50" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -6442,10 +6451,10 @@
         <v>605</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="O51" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -6469,7 +6478,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="K52" s="6" t="s">
         <v>646</v>
@@ -6506,7 +6515,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>797</v>
@@ -6543,7 +6552,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="K54" s="3" t="s">
         <v>584</v>
@@ -6581,7 +6590,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K55" s="3" t="s">
         <v>583</v>
@@ -6619,7 +6628,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>585</v>
@@ -6657,7 +6666,7 @@
         <v>1</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>583</v>
@@ -6696,7 +6705,7 @@
         <v>1</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>646</v>
@@ -6705,10 +6714,10 @@
         <v>605</v>
       </c>
       <c r="N58" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="O58" t="s">
         <v>948</v>
-      </c>
-      <c r="O58" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -6734,7 +6743,7 @@
         <v>1</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K59" s="3" t="s">
         <v>774</v>
@@ -6743,10 +6752,10 @@
         <v>605</v>
       </c>
       <c r="N59" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="O59" t="s">
         <v>950</v>
-      </c>
-      <c r="O59" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -6772,7 +6781,7 @@
         <v>1</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>774</v>
@@ -6781,10 +6790,10 @@
         <v>605</v>
       </c>
       <c r="N60" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="O60" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -6810,7 +6819,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K61" s="3" t="s">
         <v>629</v>
@@ -6819,10 +6828,10 @@
         <v>605</v>
       </c>
       <c r="N61" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="O61" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -6844,10 +6853,10 @@
         <v>605</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="O62" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -6869,10 +6878,10 @@
         <v>605</v>
       </c>
       <c r="N63" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="O63" t="s">
         <v>957</v>
-      </c>
-      <c r="O63" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -6902,10 +6911,10 @@
         <v>605</v>
       </c>
       <c r="N64" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="O64" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="136" x14ac:dyDescent="0.2">
@@ -6927,10 +6936,10 @@
         <v>605</v>
       </c>
       <c r="N65" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="O65" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -7042,10 +7051,10 @@
         <v>0</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="O68" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -7080,10 +7089,10 @@
         <v>0</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="O69" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -7118,10 +7127,10 @@
         <v>0</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="O70" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -7156,10 +7165,10 @@
         <v>0</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="O71" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -7505,10 +7514,10 @@
         <v>0</v>
       </c>
       <c r="N80" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="O80" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -7543,10 +7552,10 @@
         <v>0</v>
       </c>
       <c r="N81" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="O81" t="s">
         <v>973</v>
-      </c>
-      <c r="O81" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -7607,10 +7616,10 @@
         <v>605</v>
       </c>
       <c r="N83" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -7640,10 +7649,10 @@
         <v>605</v>
       </c>
       <c r="N84" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="O84" s="1" t="s">
         <v>975</v>
-      </c>
-      <c r="O84" s="1" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7906,10 +7915,10 @@
         <v>0</v>
       </c>
       <c r="N91" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="O91" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="92" spans="1:15" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -8029,10 +8038,10 @@
         <v>0</v>
       </c>
       <c r="N94" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="O94" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="289" x14ac:dyDescent="0.2">
@@ -8067,10 +8076,10 @@
         <v>0</v>
       </c>
       <c r="N95" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="O95" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="289" x14ac:dyDescent="0.2">
@@ -8105,10 +8114,10 @@
         <v>0</v>
       </c>
       <c r="N96" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="O96" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="97" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -8138,10 +8147,10 @@
         <v>605</v>
       </c>
       <c r="N97" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="O97" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="98" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -8174,10 +8183,10 @@
         <v>605</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="O98" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -8376,7 +8385,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
@@ -8417,7 +8426,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
@@ -8458,7 +8467,7 @@
         <v>1</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
@@ -8855,10 +8864,10 @@
         <v>605</v>
       </c>
       <c r="N116" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O116" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="117" spans="1:38" ht="34" x14ac:dyDescent="0.2">
@@ -8880,10 +8889,10 @@
         <v>605</v>
       </c>
       <c r="N117" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="O117" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="118" spans="1:38" ht="170" x14ac:dyDescent="0.2">
@@ -8908,10 +8917,10 @@
         <v>605</v>
       </c>
       <c r="N118" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="O118" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="119" spans="1:38" ht="85" x14ac:dyDescent="0.2">
@@ -9071,7 +9080,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K123" s="3" t="s">
         <v>601</v>
@@ -10148,10 +10157,10 @@
         <v>605</v>
       </c>
       <c r="N143" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="O143" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P143" s="5"/>
       <c r="Q143" s="5"/>
@@ -10208,10 +10217,10 @@
         <v>605</v>
       </c>
       <c r="N144" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="O144" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="P144" s="5"/>
       <c r="Q144" s="5"/>
@@ -10268,10 +10277,10 @@
         <v>605</v>
       </c>
       <c r="N145" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="O145" t="s">
         <v>1001</v>
-      </c>
-      <c r="O145" t="s">
-        <v>1002</v>
       </c>
       <c r="P145" s="5"/>
       <c r="Q145" s="5"/>
@@ -10320,7 +10329,7 @@
         <v>1</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K146" s="3" t="s">
         <v>601</v>
@@ -10455,10 +10464,10 @@
         <v>605</v>
       </c>
       <c r="N150" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="O150" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="151" spans="1:38" ht="68" x14ac:dyDescent="0.2">
@@ -10516,10 +10525,10 @@
         <v>605</v>
       </c>
       <c r="N152" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="O152" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="153" spans="1:38" ht="153" x14ac:dyDescent="0.2">
@@ -10541,10 +10550,10 @@
         <v>605</v>
       </c>
       <c r="N153" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="O153" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="154" spans="1:38" ht="34" x14ac:dyDescent="0.2">
@@ -10574,10 +10583,10 @@
         <v>605</v>
       </c>
       <c r="N154" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="O154" t="s">
         <v>1009</v>
-      </c>
-      <c r="O154" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="155" spans="1:38" ht="153" x14ac:dyDescent="0.2">
@@ -10599,10 +10608,10 @@
         <v>605</v>
       </c>
       <c r="N155" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="O155" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="156" spans="1:38" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -10637,10 +10646,10 @@
         <v>604</v>
       </c>
       <c r="N156" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="O156" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="157" spans="1:38" ht="85" x14ac:dyDescent="0.2">
@@ -10675,10 +10684,10 @@
         <v>604</v>
       </c>
       <c r="N157" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="O157" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="158" spans="1:38" ht="221" x14ac:dyDescent="0.2">
@@ -10713,10 +10722,10 @@
         <v>604</v>
       </c>
       <c r="N158" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="O158" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="159" spans="1:38" ht="238" x14ac:dyDescent="0.2">
@@ -10751,10 +10760,10 @@
         <v>604</v>
       </c>
       <c r="N159" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="O159" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="160" spans="1:38" ht="153" x14ac:dyDescent="0.2">
@@ -10789,10 +10798,10 @@
         <v>604</v>
       </c>
       <c r="N160" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="O160" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="161" spans="1:15" ht="119" x14ac:dyDescent="0.2">
@@ -12782,7 +12791,7 @@
         <v>1</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K219" s="3" t="s">
         <v>726</v>
@@ -12814,7 +12823,7 @@
         <v>1</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K220" s="3" t="s">
         <v>726</v>
@@ -13167,10 +13176,10 @@
         <v>0.01</v>
       </c>
       <c r="H231" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I231" s="3" t="s">
         <v>945</v>
-      </c>
-      <c r="I231" s="3" t="s">
-        <v>946</v>
       </c>
       <c r="K231" s="3" t="s">
         <v>674</v>
@@ -13462,102 +13471,102 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>